<commit_message>
signup service fully working
</commit_message>
<xml_diff>
--- a/user_candidate.xlsx
+++ b/user_candidate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14730"/>
+    <workbookView windowWidth="12705" windowHeight="14550"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>email</t>
   </si>
@@ -31,10 +31,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>40cddbfe-f044-45a8-8466-25f5fafdb6d1@mailslurp.net</t>
-  </si>
-  <si>
-    <t>40cddbfe-f044-45a8-8466-25f5fafdb6d1</t>
+    <t>5c2a7826-bbf4-4bc7-bf59-095eb60e2a7e@mailslurp.net</t>
+  </si>
+  <si>
+    <t>5c2a7826-bbf4-4bc7-bf59-095eb60e2a7e</t>
   </si>
   <si>
     <t>Jadun</t>
@@ -46,40 +46,40 @@
     <t>Larahost1!</t>
   </si>
   <si>
-    <t>fd57d8a3-5a16-4a8c-9c79-350659373a73@mailslurp.net</t>
-  </si>
-  <si>
-    <t>fd57d8a3-5a16-4a8c-9c79-350659373a73</t>
+    <t>1106ad90-d4a8-43d9-8491-888273aaf8d1@mailslurp.net</t>
+  </si>
+  <si>
+    <t>1106ad90-d4a8-43d9-8491-888273aaf8d1</t>
   </si>
   <si>
     <t>Junar</t>
   </si>
   <si>
-    <t>Lin</t>
+    <t>LinDoe</t>
   </si>
   <si>
     <t>JunarAprilLin1!</t>
   </si>
   <si>
-    <t>d8afdd9e-c6d7-4866-8bc4-4e58b37d25af@mailslurp.net</t>
-  </si>
-  <si>
-    <t>d8afdd9e-c6d7-4866-8bc4-4e58b37d25af</t>
+    <t>7186d82d-d436-4d19-8ae1-41a5fbcb17c8@mailslurp.net</t>
+  </si>
+  <si>
+    <t>7186d82d-d436-4d19-8ae1-41a5fbcb17c8</t>
   </si>
   <si>
     <t>Billy</t>
   </si>
   <si>
-    <t>Lim</t>
+    <t>LimDoe</t>
   </si>
   <si>
     <t>MaskotJakarta1!</t>
   </si>
   <si>
-    <t>0d5c4317-9e16-4f94-80ad-3fd5971977aa@mailslurp.net</t>
-  </si>
-  <si>
-    <t>0d5c4317-9e16-4f94-80ad-3fd5971977aa</t>
+    <t>38984ee7-4b30-4681-8982-6a10144a1c61@mailslurp.net</t>
+  </si>
+  <si>
+    <t>38984ee7-4b30-4681-8982-6a10144a1c61</t>
   </si>
   <si>
     <t>Lunar</t>
@@ -91,10 +91,10 @@
     <t>UbuntuJurnal1!</t>
   </si>
   <si>
-    <t>056c018f-1449-4806-a89b-a7aad97f6f19@mailslurp.net</t>
-  </si>
-  <si>
-    <t>056c018f-1449-4806-a89b-a7aad97f6f19</t>
+    <t>c9369e67-8a44-4946-b7ec-2b5e2311decc@mailslurp.net</t>
+  </si>
+  <si>
+    <t>c9369e67-8a44-4946-b7ec-2b5e2311decc</t>
   </si>
   <si>
     <t>JoshBus</t>
@@ -104,6 +104,51 @@
   </si>
   <si>
     <t>JbMate011!</t>
+  </si>
+  <si>
+    <t>0eecb53e-7ecb-4305-ba02-d374a5735b8f@mailslurp.net</t>
+  </si>
+  <si>
+    <t>0eecb53e-7ecb-4305-ba02-d374a5735b8f</t>
+  </si>
+  <si>
+    <t>Holly</t>
+  </si>
+  <si>
+    <t>Balai</t>
+  </si>
+  <si>
+    <t>MatetoStar1!</t>
+  </si>
+  <si>
+    <t>2dac5c6c-f1d1-440b-a6bb-d4ca90ebf70b@mailslurp.net</t>
+  </si>
+  <si>
+    <t>2dac5c6c-f1d1-440b-a6bb-d4ca90ebf70b</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>Rash</t>
+  </si>
+  <si>
+    <t>KliniGus1!</t>
+  </si>
+  <si>
+    <t>859c0ceb-1173-4683-81e0-76152ef3a9d2@mailslurp.net</t>
+  </si>
+  <si>
+    <t>859c0ceb-1173-4683-81e0-76152ef3a9d2</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Wahlberg</t>
+  </si>
+  <si>
+    <t>Matroska1!</t>
   </si>
 </sst>
 </file>
@@ -111,10 +156,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -134,22 +179,98 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,78 +284,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,21 +300,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,19 +323,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -302,163 +479,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,7 +536,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,17 +556,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,31 +600,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,144 +619,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,12 +764,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1048,13 +1096,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="50" customWidth="1"/>
     <col min="2" max="2" width="44.625" customWidth="1"/>
@@ -1084,7 +1132,7 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
@@ -1101,7 +1149,7 @@
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
@@ -1152,7 +1200,7 @@
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C6" t="s">
@@ -1163,15 +1211,69 @@
       </c>
       <c r="E6" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="40cddbfe-f044-45a8-8466-25f5fafdb6d1@mailslurp.net" tooltip="mailto:40cddbfe-f044-45a8-8466-25f5fafdb6d1@mailslurp.net"/>
-    <hyperlink ref="A3" r:id="rId2" display="fd57d8a3-5a16-4a8c-9c79-350659373a73@mailslurp.net"/>
-    <hyperlink ref="A4" r:id="rId3" display="d8afdd9e-c6d7-4866-8bc4-4e58b37d25af@mailslurp.net"/>
-    <hyperlink ref="A5" r:id="rId4" display="0d5c4317-9e16-4f94-80ad-3fd5971977aa@mailslurp.net"/>
-    <hyperlink ref="A6" r:id="rId5" display="056c018f-1449-4806-a89b-a7aad97f6f19@mailslurp.net"/>
+    <hyperlink ref="A2" r:id="rId1" display="5c2a7826-bbf4-4bc7-bf59-095eb60e2a7e@mailslurp.net"/>
+    <hyperlink ref="A3" r:id="rId2" display="1106ad90-d4a8-43d9-8491-888273aaf8d1@mailslurp.net"/>
+    <hyperlink ref="A4" r:id="rId3" display="7186d82d-d436-4d19-8ae1-41a5fbcb17c8@mailslurp.net"/>
+    <hyperlink ref="A5" r:id="rId4" display="38984ee7-4b30-4681-8982-6a10144a1c61@mailslurp.net"/>
+    <hyperlink ref="A6" r:id="rId5" display="c9369e67-8a44-4946-b7ec-2b5e2311decc@mailslurp.net"/>
+    <hyperlink ref="A7" r:id="rId6" display="0eecb53e-7ecb-4305-ba02-d374a5735b8f@mailslurp.net"/>
+    <hyperlink ref="A8" r:id="rId7" display="2dac5c6c-f1d1-440b-a6bb-d4ca90ebf70b@mailslurp.net"/>
+    <hyperlink ref="A9" r:id="rId8" display="859c0ceb-1173-4683-81e0-76152ef3a9d2@mailslurp.net"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
chore: remove unused line
</commit_message>
<xml_diff>
--- a/user_candidate.xlsx
+++ b/user_candidate.xlsx
@@ -55,10 +55,10 @@
     <t>adress</t>
   </si>
   <si>
-    <t>ff74b806-d326-4795-9576-0a42d9a86e71@mailslurp.net</t>
-  </si>
-  <si>
-    <t>ff74b806-d326-4795-9576-0a42d9a86e71</t>
+    <t>rubiaha@outlook.com</t>
+  </si>
+  <si>
+    <t>abae4168-f59c-4435-9565-fe85d0d5ab82</t>
   </si>
   <si>
     <t>Magiss</t>
@@ -76,7 +76,7 @@
     <t>Toronto</t>
   </si>
   <si>
-    <t>82231811103</t>
+    <t>82231810103</t>
   </si>
   <si>
     <t>Software Development</t>
@@ -94,10 +94,10 @@
     <t>Unnamed Road, Sekar Putih, SekarPutih, Bagor, Nganjuk</t>
   </si>
   <si>
-    <t>cb38903d-9768-49b8-8793-22409b897521@mailslurp.net</t>
-  </si>
-  <si>
-    <t>cb38903d-9768-49b8-8793-22409b897521</t>
+    <t>jericatlima@outlook.com</t>
+  </si>
+  <si>
+    <t>abae4168-f59c-4435-9565-fe85d0d5ab81</t>
   </si>
   <si>
     <t>Koala</t>
@@ -112,13 +112,13 @@
     <t>Jakarta</t>
   </si>
   <si>
-    <t>82231811102</t>
-  </si>
-  <si>
-    <t>44a94cd3-3307-40b7-8d27-08321627080a@mailslurp.net</t>
-  </si>
-  <si>
-    <t>44a94cd3-3307-40b7-8d27-08321627080a</t>
+    <t>82231810102</t>
+  </si>
+  <si>
+    <t>chibicapa@outlook.com</t>
+  </si>
+  <si>
+    <t>abae4168-f59c-4435-9565-fe85d0d5ab83</t>
   </si>
   <si>
     <t>Mongking</t>
@@ -130,13 +130,13 @@
     <t>Surabaya</t>
   </si>
   <si>
-    <t>82231811104</t>
-  </si>
-  <si>
-    <t>6ddea427-840b-4653-a1bb-c58127de84a2@mailslurp.net</t>
-  </si>
-  <si>
-    <t>6ddea427-840b-4653-a1bb-c58127de84a2</t>
+    <t>82231810104</t>
+  </si>
+  <si>
+    <t>radiandrive@gmail.com</t>
+  </si>
+  <si>
+    <t>abae4168-f59c-4435-9565-fe85d0d5ab84</t>
   </si>
   <si>
     <t>Hilman</t>
@@ -151,13 +151,13 @@
     <t>Warsaw</t>
   </si>
   <si>
-    <t>82231811105</t>
-  </si>
-  <si>
-    <t>faa90c79-ede5-40f5-834d-cb815429e3d9@mailslurp.net</t>
-  </si>
-  <si>
-    <t>faa90c79-ede5-40f5-834d-cb815429e3d9</t>
+    <t>82231810105</t>
+  </si>
+  <si>
+    <t>dhiandrive@gmail.com</t>
+  </si>
+  <si>
+    <t>abae4168-f59c-4435-9565-fe85d0d5ab85</t>
   </si>
   <si>
     <t>Maili</t>
@@ -172,7 +172,7 @@
     <t>Kyiv</t>
   </si>
   <si>
-    <t>82231811106</t>
+    <t>82231810106</t>
   </si>
 </sst>
 </file>
@@ -180,10 +180,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -209,9 +209,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -225,90 +278,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -322,17 +330,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -353,181 +353,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -538,6 +538,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -555,21 +570,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,13 +604,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -624,17 +628,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -643,139 +643,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1123,7 +1123,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5"/>
@@ -1390,11 +1390,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="ff74b806-d326-4795-9576-0a42d9a86e71@mailslurp.net" tooltip="mailto:ff74b806-d326-4795-9576-0a42d9a86e71@mailslurp.net"/>
-    <hyperlink ref="A4" r:id="rId2" display="44a94cd3-3307-40b7-8d27-08321627080a@mailslurp.net" tooltip="mailto:44a94cd3-3307-40b7-8d27-08321627080a@mailslurp.net"/>
-    <hyperlink ref="A6" r:id="rId3" display="faa90c79-ede5-40f5-834d-cb815429e3d9@mailslurp.net" tooltip="mailto:faa90c79-ede5-40f5-834d-cb815429e3d9@mailslurp.net"/>
-    <hyperlink ref="A5" r:id="rId4" display="6ddea427-840b-4653-a1bb-c58127de84a2@mailslurp.net" tooltip="mailto:6ddea427-840b-4653-a1bb-c58127de84a2@mailslurp.net"/>
-    <hyperlink ref="A3" r:id="rId5" display="cb38903d-9768-49b8-8793-22409b897521@mailslurp.net" tooltip="mailto:cb38903d-9768-49b8-8793-22409b897521@mailslurp.net"/>
+    <hyperlink ref="A2" r:id="rId1" display="rubiaha@outlook.com" tooltip="mailto:rubiaha@outlook.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="chibicapa@outlook.com" tooltip="mailto:chibicapa@outlook.com"/>
+    <hyperlink ref="A6" r:id="rId3" display="dhiandrive@gmail.com"/>
+    <hyperlink ref="A5" r:id="rId4" display="radiandrive@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId5" display="jericatlima@outlook.com" tooltip="mailto:jericatlima@outlook.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>